<commit_message>
Made changes to the FHQ test scripts
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/FHQScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/FHQScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83ADB5D-2A59-C641-AE6B-FB9617212DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796A4A72-FCC8-2742-87B9-D76C31087A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="500" windowWidth="18660" windowHeight="20280" activeTab="15" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
+    <workbookView xWindow="1780" yWindow="500" windowWidth="18660" windowHeight="20280" firstSheet="10" activeTab="14" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3325" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3336" uniqueCount="430">
   <si>
     <t>Question</t>
   </si>
@@ -1332,6 +1332,15 @@
   </si>
   <si>
     <t>FHQ Aunt/Uncle: ParticipantAuntFirstName…</t>
+  </si>
+  <si>
+    <t>Aunt/Uncle First Initial of LAST Name Value</t>
+  </si>
+  <si>
+    <t>Aunt/Uncle Vital Status Value</t>
+  </si>
+  <si>
+    <t>Aunt/Uncle First Name Value</t>
   </si>
 </sst>
 </file>
@@ -7087,8 +7096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90F0027-F00B-1B4B-AE3D-053640C4AD50}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -7980,7 +7989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686FEE5D-0F02-AC40-AA06-77804C89CACF}">
   <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
@@ -13126,10 +13135,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440C8FC-FCC1-A240-91E3-288B715C9C66}">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -13289,7 +13298,7 @@
         <v>409</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13297,7 +13306,7 @@
         <v>410</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13318,209 +13327,209 @@
         <v>295</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>6</v>
+        <v>429</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>401</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>260</v>
+        <v>427</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>260</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>261</v>
+        <v>428</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>413</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>87</v>
+        <v>261</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="132" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>90</v>
+        <v>413</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1900</v>
+        <v>266</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="132" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="37" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="43" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="44" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    <row r="45" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="46" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+    <row r="47" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B50" s="3">
         <v>1</v>
@@ -13528,559 +13537,583 @@
     </row>
     <row r="51" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+    <row r="59" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+    <row r="60" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+    <row r="61" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+    <row r="62" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>175</v>
+        <v>73</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B70" s="3">
-        <v>1900</v>
+        <v>173</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
+    <row r="76" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+    <row r="77" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+    <row r="78" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+    <row r="79" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B81" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="82" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B82" s="3">
-        <v>1900</v>
+        <v>166</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B83" s="3"/>
+        <v>181</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="84" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="94" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+    <row r="97" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B97" s="3">
         <v>1900</v>
       </c>
     </row>
-    <row r="95" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+    <row r="98" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+    <row r="100" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+    <row r="101" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B101" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="66" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
+    <row r="102" spans="1:2" ht="66" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+    <row r="103" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="105" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>424</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>403</v>
+        <v>72</v>
       </c>
     </row>
     <row r="109" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+    <row r="114" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
+    <row r="115" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="113" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
+    <row r="116" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="114" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
+    <row r="117" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>397</v>
+        <v>47</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>336</v>
+        <v>47</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>416</v>
+        <v>394</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B124" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -14091,10 +14124,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A1A7AA-D469-814C-86B3-A8D7D6B424B5}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A20" sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -14244,6 +14277,9 @@
       <c r="A18" s="3" t="s">
         <v>408</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -14281,221 +14317,215 @@
       <c r="A23" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>336</v>
-      </c>
     </row>
     <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>6</v>
+        <v>429</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>401</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>260</v>
+        <v>427</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>260</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>261</v>
+        <v>428</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>413</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>87</v>
+        <v>261</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="132" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>90</v>
+        <v>413</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1900</v>
+        <v>266</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="132" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="37" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="43" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="44" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    <row r="45" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="46" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+    <row r="47" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B50" s="3">
         <v>1</v>
@@ -14503,559 +14533,583 @@
     </row>
     <row r="51" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" s="5" customFormat="1" ht="132" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="5" customFormat="1" ht="132" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+    <row r="59" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+    <row r="60" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+    <row r="61" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+    <row r="62" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>175</v>
+        <v>73</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B70" s="3">
-        <v>1900</v>
+        <v>173</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
+    <row r="76" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+    <row r="77" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+    <row r="78" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+    <row r="79" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B81" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="82" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B82" s="3">
-        <v>1900</v>
+        <v>166</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B83" s="3"/>
+        <v>181</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="84" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="94" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+    <row r="97" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B97" s="3">
         <v>1900</v>
       </c>
     </row>
-    <row r="95" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+    <row r="98" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+    <row r="100" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+    <row r="101" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B101" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="66" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
+    <row r="102" spans="1:2" ht="66" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+    <row r="103" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="105" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>425</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>340</v>
+        <v>72</v>
       </c>
     </row>
     <row r="109" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+    <row r="114" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
+    <row r="115" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="113" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
+    <row r="116" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="114" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
+    <row r="117" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>397</v>
+        <v>47</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>336</v>
+        <v>47</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>416</v>
+        <v>394</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B124" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15068,8 +15122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C165AD-8F20-F342-8EE0-C1843FC10E3A}">
   <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView topLeftCell="A19" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -15314,7 +15368,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="88" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="110" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Made changes to FHQ files based on new child RP scenario
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/FHQScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/FHQScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFF0712-16E7-984D-A236-07FED6968BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CCB7FC-6E05-D442-B559-AD39BB34544D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17580" activeTab="4" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
+    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17580" activeTab="7" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant" sheetId="4" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3624" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3624" uniqueCount="471">
   <si>
     <t>Question</t>
   </si>
@@ -1386,9 +1386,6 @@
   </si>
   <si>
     <t>Please enter one record per each family member for whom you have knowledge.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter one record per each family member for whom you have knowledge. </t>
   </si>
   <si>
     <t>Please make sure you have completed all Sibling records before completing Niece/Nephew records. You can use the blue “Back to Home” button to return and edit the Sibling records if needed.</t>
@@ -2031,7 +2028,7 @@
         <v>428</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -2095,7 +2092,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -2111,7 +2108,7 @@
         <v>371</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -2519,7 +2516,7 @@
         <v>373</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -3327,7 +3324,7 @@
         <v>409</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -4358,7 +4355,7 @@
         <v>409</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -5385,7 +5382,7 @@
         <v>409</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -5827,7 +5824,7 @@
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>284</v>
@@ -6430,7 +6427,7 @@
         <v>409</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -6847,7 +6844,7 @@
         <v>210</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -6895,10 +6892,10 @@
     </row>
     <row r="29" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -7386,7 +7383,7 @@
         <v>409</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -7815,10 +7812,10 @@
     </row>
     <row r="21" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -7845,7 +7842,7 @@
     </row>
     <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B25" s="3"/>
     </row>
@@ -7867,10 +7864,10 @@
     </row>
     <row r="28" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -7889,7 +7886,7 @@
     </row>
     <row r="31" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>310</v>
@@ -7897,7 +7894,7 @@
     </row>
     <row r="32" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B32" s="3"/>
     </row>
@@ -7922,7 +7919,7 @@
         <v>210</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -7975,10 +7972,10 @@
     </row>
     <row r="42" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>446</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -8466,7 +8463,7 @@
         <v>409</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -9454,7 +9451,7 @@
         <v>409</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="96" spans="1:2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -9946,7 +9943,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -10354,7 +10351,7 @@
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>105</v>
@@ -10865,7 +10862,7 @@
         <v>409</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -11902,7 +11899,7 @@
         <v>409</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -12228,8 +12225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3F8D73-A2F8-A34D-BAA9-8CA076BBD188}">
   <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -12539,18 +12536,18 @@
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
@@ -12571,10 +12568,10 @@
     </row>
     <row r="43" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -12587,7 +12584,7 @@
     </row>
     <row r="45" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>361</v>
@@ -12982,7 +12979,7 @@
         <v>409</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13985,7 +13982,7 @@
         <v>409</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -14988,7 +14985,7 @@
         <v>409</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -15355,8 +15352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A1A7AA-D469-814C-86B3-A8D7D6B424B5}">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -15605,7 +15602,7 @@
         <v>443</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -16061,7 +16058,7 @@
         <v>409</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -16605,7 +16602,7 @@
         <v>210</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -16652,10 +16649,10 @@
     </row>
     <row r="28" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -17111,7 +17108,7 @@
         <v>409</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="44" x14ac:dyDescent="0.2">

</xml_diff>